<commit_message>
Fixing EDD-920 failing test in combinatorial creation file code
</commit_message>
<xml_diff>
--- a/main/static/main/example/sample_experiment_description.xlsx
+++ b/main/static/main/example/sample_experiment_description.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12220" yWindow="4480" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="simple_template_file.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Line Name</t>
   </si>
@@ -33,6 +33,9 @@
     <t>Media</t>
   </si>
   <si>
+    <t>Metabolomics Time(s)</t>
+  </si>
+  <si>
     <t>181-aceF</t>
   </si>
   <si>
@@ -42,17 +45,26 @@
     <t>LB</t>
   </si>
   <si>
+    <t>8h, 24h</t>
+  </si>
+  <si>
+    <t>4h, 6h</t>
+  </si>
+  <si>
+    <t>Targeted Proteomics Time(s)</t>
+  </si>
+  <si>
+    <t>Description blah blah</t>
+  </si>
+  <si>
     <t>Part ID</t>
-  </si>
-  <si>
-    <t>Describe your line here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -76,27 +88,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,9 +115,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -457,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -468,41 +465,54 @@
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
-        <v>3</v>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted changes to the example file, and fixed underlying file naming / testing TODO's that caused the reversion 1) Reverted changes to the sample file intended for users 2) Reverted change to the ED unit test that caused it to reference the sample file intended for users. 3) Renamed file intended as test input to clarify the difference. 4) Implemented TODO in the unit test that makes it now dependent on the advanced ED file as intended / as manually tested before the ED feature got released around the holidays
</commit_message>
<xml_diff>
--- a/main/static/main/example/sample_experiment_description.xlsx
+++ b/main/static/main/example/sample_experiment_description.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="12220" yWindow="4480" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="simple_template_file.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Line Name</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Media</t>
   </si>
   <si>
-    <t>Metabolomics Time(s)</t>
-  </si>
-  <si>
     <t>181-aceF</t>
   </si>
   <si>
@@ -45,26 +42,17 @@
     <t>LB</t>
   </si>
   <si>
-    <t>8h, 24h</t>
-  </si>
-  <si>
-    <t>4h, 6h</t>
-  </si>
-  <si>
-    <t>Targeted Proteomics Time(s)</t>
-  </si>
-  <si>
-    <t>Description blah blah</t>
-  </si>
-  <si>
     <t>Part ID</t>
+  </si>
+  <si>
+    <t>Describe your line here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,13 +76,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -115,8 +117,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -454,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -465,54 +468,41 @@
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
+      <c r="E2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>